<commit_message>
Correct csproj file tags and url value
</commit_message>
<xml_diff>
--- a/Test/UnitTest/srcTest/simpleGeneric.xlsx
+++ b/Test/UnitTest/srcTest/simpleGeneric.xlsx
@@ -12,7 +12,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2r3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3we</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3wer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34wr</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61,37 +83,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="6">
-      <c r="F6">
-        <v>34</v>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-      <c r="G6">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="H6">
-        <v>34</v>
+      <c r="C2" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="F7">
-        <v>1</v>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
       </c>
-      <c r="G7">
-        <v>55</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
-      <c r="H7">
-        <v>34354</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>4</v>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>